<commit_message>
This commit was a mistake
</commit_message>
<xml_diff>
--- a/results/merged-dataframe-cleaned.xlsx
+++ b/results/merged-dataframe-cleaned.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,95 +436,100 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>CHROM_x</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>POS_x</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>End_x</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>REF_x</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ALT_x</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Func.ensGene</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ExonicFunc.ensGene</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>AAChange.ensGene</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>avsnp150</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: Clinvar </t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>InterVar_automated</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Clin_Sig_inhouse</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Role</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Var_type</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>chrom</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>strand</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Start</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>End</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Gene name</t>
         </is>
@@ -534,62 +539,60 @@
       <c r="A2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>751</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>chr20</t>
         </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2635436</v>
       </c>
       <c r="D2" t="n">
         <v>2635436</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>2635436</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>ENSG00000101361:ENST00000329276:exon5:c.412G&gt;T:p.Asp138Tyr,ENSG00000101361:ENST00000445139:exon5:c.412G&gt;T:p.Asp138Tyr</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>rs11553608</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N2" t="inlineStr">
         <is>
           <t>.</t>
@@ -597,26 +600,31 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>chr20</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>2634857</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>2634932</v>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>SNORD110</t>
         </is>
@@ -626,89 +634,92 @@
       <c r="A3" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>733</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>chr3</t>
         </is>
-      </c>
-      <c r="C3" t="n">
-        <v>10183635</v>
       </c>
       <c r="D3" t="n">
         <v>10183635</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>10183635</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>ENSG00000134086:ENST00000256474:exon1:c.104C&gt;T:p.Ala35Val,ENSG00000134086:ENST00000345392:exon1:c.104C&gt;T:p.Ala35Val</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>rs587780536</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: Uncertain_significance </t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N3" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
           <t>TSG</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>chr3</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>10183461</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>10195351</v>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>VHL</t>
         </is>
@@ -718,62 +729,60 @@
       <c r="A4" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>749</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>chr12</t>
         </is>
-      </c>
-      <c r="C4" t="n">
-        <v>14578083</v>
       </c>
       <c r="D4" t="n">
         <v>14578083</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="n">
+        <v>14578083</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>ENSG00000171681:ENST00000540793:exon1:c.1234G&gt;A:p.Glu412Lys,ENSG00000171681:ENST00000261168:exon2:c.1234G&gt;A:p.Glu412Lys,ENSG00000171681:ENST00000396279:exon2:c.1234G&gt;A:p.Glu412Lys,ENSG00000171681:ENST00000536444:exon2:c.1234G&gt;A:p.Glu412Lys,ENSG00000171681:ENST00000543189:exon2:c.1234G&gt;A:p.Glu412Lys,ENSG00000171681:ENST00000544627:exon2:c.1258G&gt;A:p.Glu420Lys</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>rs567077220</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N4" t="inlineStr">
         <is>
           <t>.</t>
@@ -781,26 +790,31 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>chr12</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>14570901</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>14655864</v>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>ATF7IP</t>
         </is>
@@ -810,62 +824,60 @@
       <c r="A5" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>705</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>chr3</t>
         </is>
-      </c>
-      <c r="C5" t="n">
-        <v>25641017</v>
       </c>
       <c r="D5" t="n">
         <v>25641017</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="n">
+        <v>25641017</v>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>ENSG00000077097:ENST00000540199:exon11:c.1175A&gt;T:p.Lys392Ile,ENSG00000077097:ENST00000542520:exon12:c.1175A&gt;T:p.Lys392Ile,ENSG00000077097:ENST00000264331:exon35:c.4619A&gt;T:p.Lys1540Ile,ENSG00000077097:ENST00000435706:exon35:c.4604A&gt;T:p.Lys1535Ile</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N5" t="inlineStr">
         <is>
           <t>.</t>
@@ -873,26 +885,31 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>chr3</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>25639474</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>25706398</v>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>TOP2B</t>
         </is>
@@ -902,62 +919,60 @@
       <c r="A6" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="n">
+        <v>739</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>chr17</t>
         </is>
-      </c>
-      <c r="C6" t="n">
-        <v>34251695</v>
       </c>
       <c r="D6" t="n">
         <v>34251695</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" t="n">
+        <v>34251695</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>ENSG00000187456:ENST00000394529:exon3:c.412T&gt;A:p.Cys138Ser,ENSG00000187456:ENST00000419453:exon3:c.412T&gt;A:p.Cys138Ser,ENSG00000187456:ENST00000430160:exon3:c.412T&gt;A:p.Cys138Ser,ENSG00000187456:ENST00000293273:exon4:c.481T&gt;A:p.Cys161Ser,ENSG00000187456:ENST00000394528:exon4:c.481T&gt;A:p.Cys161Ser,ENSG00000187456:ENST00000431884:exon4:c.481T&gt;A:p.Cys161Ser</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="K6" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N6" t="inlineStr">
         <is>
           <t>.</t>
@@ -965,26 +980,31 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>chr17</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>34249481</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>34257303</v>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>RDM1</t>
         </is>
@@ -994,89 +1014,92 @@
       <c r="A7" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="n">
+        <v>762</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>chrX</t>
         </is>
-      </c>
-      <c r="C7" t="n">
-        <v>66765158</v>
       </c>
       <c r="D7" t="n">
         <v>66765158</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" t="n">
+        <v>66765158</v>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>ENSG00000169083:ENST00000374690:exon1:c.170T&gt;A:p.Leu57Gln,ENSG00000169083:ENST00000396044:exon1:c.170T&gt;A:p.Leu57Gln,ENSG00000169083:ENST00000504326:exon1:c.170T&gt;A:p.Leu57Gln,ENSG00000169083:ENST00000514029:exon1:c.170T&gt;A:p.Leu57Gln</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>rs78686797</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N7" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
           <t>Oncogenic</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>chrX</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="R7" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>66764464</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>66915917</v>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>AR</t>
         </is>
@@ -1086,62 +1109,60 @@
       <c r="A8" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="n">
+        <v>708</v>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>chr11</t>
         </is>
-      </c>
-      <c r="C8" t="n">
-        <v>69625359</v>
       </c>
       <c r="D8" t="n">
         <v>69625359</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" t="n">
+        <v>69625359</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>ENSG00000186895:ENST00000334134:exon3:c.434G&gt;A:p.Arg145Gln</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>rs782088765</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N8" t="inlineStr">
         <is>
           <t>.</t>
@@ -1149,26 +1170,31 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>chr11</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="R8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>69624735</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>69634184</v>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>FGF3</t>
         </is>
@@ -1178,37 +1204,35 @@
       <c r="A9" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="n">
+        <v>655</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>chr15</t>
         </is>
-      </c>
-      <c r="C9" t="n">
-        <v>90631571</v>
       </c>
       <c r="D9" t="n">
         <v>90631571</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" t="n">
+        <v>90631571</v>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="I9" t="inlineStr">
         <is>
           <t>.</t>
@@ -1221,14 +1245,14 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="M9" t="inlineStr">
         <is>
           <t>.</t>
@@ -1241,26 +1265,31 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>chr15</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>90627209</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>90643853</v>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>IDH2</t>
         </is>
@@ -1270,62 +1299,60 @@
       <c r="A10" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="n">
+        <v>745</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>chrX</t>
         </is>
-      </c>
-      <c r="C10" t="n">
-        <v>100652892</v>
       </c>
       <c r="D10" t="n">
         <v>100652892</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" t="n">
+        <v>100652892</v>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>ENSG00000102393:ENST00000218516:exon7:c.1195T&gt;A:p.Trp399Arg</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N10" t="inlineStr">
         <is>
           <t>.</t>
@@ -1333,26 +1360,31 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>chrX</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>100652790</v>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>100662913</v>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>GLA</t>
         </is>
@@ -1362,62 +1394,60 @@
       <c r="A11" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="n">
+        <v>758</v>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>chr8</t>
         </is>
-      </c>
-      <c r="C11" t="n">
-        <v>144996316</v>
       </c>
       <c r="D11" t="n">
         <v>144996316</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" t="n">
+        <v>144996316</v>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>ENSG00000178209:ENST00000322810:exon32:c.8084G&gt;A:p.Arg2695Gln,ENSG00000178209:ENST00000345136:exon32:c.7673G&gt;A:p.Arg2558Gln,ENSG00000178209:ENST00000354589:exon32:c.7673G&gt;A:p.Arg2558Gln,ENSG00000178209:ENST00000354958:exon32:c.7607G&gt;A:p.Arg2536Gln,ENSG00000178209:ENST00000356346:exon32:c.7631G&gt;A:p.Arg2544Gln,ENSG00000178209:ENST00000357649:exon32:c.7685G&gt;A:p.Arg2562Gln,ENSG00000178209:ENST00000398774:exon32:c.7577G&gt;A:p.Arg2526Gln,ENSG00000178209:ENST00000527096:exon32:c.7742G&gt;A:p.Arg2581Gln,ENSG00000178209:ENST00000436759:exon33:c.7754G&gt;A:p.Arg2585Gln</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>rs782713454</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N11" t="inlineStr">
         <is>
           <t>.</t>
@@ -1425,26 +1455,31 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>chr8</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>144989320</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>145018938</v>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>PLEC</t>
         </is>
@@ -1454,89 +1489,92 @@
       <c r="A12" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="n">
+        <v>748</v>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>chr5</t>
         </is>
-      </c>
-      <c r="C12" t="n">
-        <v>149509379</v>
       </c>
       <c r="D12" t="n">
         <v>149509379</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" t="n">
+        <v>149509379</v>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>ENSG00000113721:ENST00000261799:exon10:c.1520G&gt;A:p.Arg507His</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>rs145823245</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>LIKELY_BENIGN</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N12" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
           <t>Oncogenic</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>chr5</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>149493401</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>149535408</v>
       </c>
-      <c r="T12" t="inlineStr">
+      <c r="U12" t="inlineStr">
         <is>
           <t>PDGFRB</t>
         </is>
@@ -1546,37 +1584,35 @@
       <c r="A13" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="n">
+        <v>690</v>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>chr7</t>
         </is>
-      </c>
-      <c r="C13" t="n">
-        <v>155592941</v>
       </c>
       <c r="D13" t="n">
         <v>155592941</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" t="n">
+        <v>155592941</v>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>splicing</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="I13" t="inlineStr">
         <is>
           <t>.</t>
@@ -1589,14 +1625,14 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="M13" t="inlineStr">
         <is>
           <t>.</t>
@@ -1609,26 +1645,31 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>chr7</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="R13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R13" t="n">
+      <c r="S13" t="n">
         <v>155592673</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>155605157</v>
       </c>
-      <c r="T13" t="inlineStr">
+      <c r="U13" t="inlineStr">
         <is>
           <t>SHH</t>
         </is>
@@ -1638,89 +1679,92 @@
       <c r="A14" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="n">
+        <v>763</v>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>chr5</t>
         </is>
-      </c>
-      <c r="C14" t="n">
-        <v>176637090</v>
       </c>
       <c r="D14" t="n">
         <v>176637090</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" t="n">
+        <v>176637090</v>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>ENSG00000165671:ENST00000361032:exon2:c.1381G&gt;A:p.Ala461Thr,ENSG00000165671:ENST00000439151:exon5:c.1690G&gt;A:p.Ala564Thr,ENSG00000165671:ENST00000347982:exon6:c.883G&gt;A:p.Ala295Thr,ENSG00000165671:ENST00000354179:exon6:c.883G&gt;A:p.Ala295Thr</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="K14" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N14" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
           <t>TSG/Oncogenic</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>chr5</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
         <v>176561229</v>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>176727214</v>
       </c>
-      <c r="T14" t="inlineStr">
+      <c r="U14" t="inlineStr">
         <is>
           <t>NSD1</t>
         </is>
@@ -1730,62 +1774,60 @@
       <c r="A15" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" t="n">
+        <v>712</v>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>chr4</t>
         </is>
-      </c>
-      <c r="C15" t="n">
-        <v>187516969</v>
       </c>
       <c r="D15" t="n">
         <v>187516969</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" t="n">
+        <v>187516969</v>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>ENSG00000083857:ENST00000441802:exon26:c.13012G&gt;T:p.Asp4338Tyr</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="K15" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N15" t="inlineStr">
         <is>
           <t>.</t>
@@ -1793,26 +1835,31 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>chr4</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="R15" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>187508947</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>187645010</v>
       </c>
-      <c r="T15" t="inlineStr">
+      <c r="U15" t="inlineStr">
         <is>
           <t>FAT1</t>
         </is>
@@ -1822,62 +1869,60 @@
       <c r="A16" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" t="n">
+        <v>736</v>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>chr4</t>
         </is>
-      </c>
-      <c r="C16" t="n">
-        <v>187524933</v>
       </c>
       <c r="D16" t="n">
         <v>187524933</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" t="n">
+        <v>187524933</v>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>ENSG00000083857:ENST00000441802:exon19:c.10747G&gt;A:p.Asp3583Asn</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>rs749223648</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N16" t="inlineStr">
         <is>
           <t>.</t>
@@ -1885,26 +1930,31 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>chr4</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="R16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
         <v>187508947</v>
       </c>
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>187645010</v>
       </c>
-      <c r="T16" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>FAT1</t>
         </is>
@@ -1914,62 +1964,60 @@
       <c r="A17" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" t="n">
+        <v>761</v>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>chr2</t>
         </is>
-      </c>
-      <c r="C17" t="n">
-        <v>209106843</v>
       </c>
       <c r="D17" t="n">
         <v>209106843</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E17" t="n">
+        <v>209106843</v>
+      </c>
+      <c r="F17" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>exonic</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>Nonsynonymous SNV</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>ENSG00000138413:ENST00000345146:exon7:c.725A&gt;T:p.Gln242Leu,ENSG00000138413:ENST00000415913:exon7:c.725A&gt;T:p.Gln242Leu,ENSG00000138413:ENST00000446179:exon7:c.725A&gt;T:p.Gln242Leu</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="K17" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t xml:space="preserve">clinvar: UNK </t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>UNCERTAIN_SIGNIFICANCE</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
       <c r="N17" t="inlineStr">
         <is>
           <t>.</t>
@@ -1977,26 +2025,31 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
           <t>SNV</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>chr2</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
+      <c r="R17" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
         <v>209100952</v>
       </c>
-      <c r="S17" t="n">
+      <c r="T17" t="n">
         <v>209119795</v>
       </c>
-      <c r="T17" t="inlineStr">
+      <c r="U17" t="inlineStr">
         <is>
           <t>IDH1</t>
         </is>

</xml_diff>